<commit_message>
Developing Actions code for dropdowns
</commit_message>
<xml_diff>
--- a/src/main/resources/Testdatas/VendoTestdatas.xlsx
+++ b/src/main/resources/Testdatas/VendoTestdatas.xlsx
@@ -244,9 +244,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -277,6 +277,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -285,10 +300,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -299,8 +331,61 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -314,84 +399,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -401,14 +408,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -429,31 +429,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -465,151 +597,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -651,6 +651,30 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -662,6 +686,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -690,30 +723,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -731,15 +740,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -751,15 +751,15 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -769,130 +769,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1265,8 +1265,8 @@
   <sheetPr/>
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="6"/>

</xml_diff>

<commit_message>
code is optimized scroll function is pending
</commit_message>
<xml_diff>
--- a/src/main/resources/Testdatas/VendoTestdatas.xlsx
+++ b/src/main/resources/Testdatas/VendoTestdatas.xlsx
@@ -214,7 +214,7 @@
     <t>xpath = //android.widget.EditText[@text='Pan No']</t>
   </si>
   <si>
-    <t>3WEKY5JOR4</t>
+    <t>AERPE9129F</t>
   </si>
   <si>
     <t>Pan Image</t>
@@ -229,7 +229,7 @@
     <t>Terms &amp; Conditions</t>
   </si>
   <si>
-    <t>xpath = //android.widget.CheckBox[16]</t>
+    <t>className = android.widget.CheckBox</t>
   </si>
   <si>
     <t>Continue</t>
@@ -243,10 +243,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -277,10 +277,58 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -292,38 +340,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -347,45 +363,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -399,6 +378,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -408,6 +394,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -429,187 +429,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -651,11 +651,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -671,6 +677,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -699,15 +714,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -723,21 +729,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -748,10 +739,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -763,136 +766,133 @@
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1265,8 +1265,8 @@
   <sheetPr/>
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="6"/>

</xml_diff>

<commit_message>
Appium server staring code is implemented
</commit_message>
<xml_diff>
--- a/src/main/resources/Testdatas/VendoTestdatas.xlsx
+++ b/src/main/resources/Testdatas/VendoTestdatas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="77">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -61,7 +61,7 @@
     <t>Enter</t>
   </si>
   <si>
-    <t>Ezhil</t>
+    <t>Karthick</t>
   </si>
   <si>
     <t>Enter Lastname</t>
@@ -88,7 +88,7 @@
     <t>xpath = //android.widget.EditText[@text='Mobile Number*']</t>
   </si>
   <si>
-    <t>6385654526</t>
+    <t>9962648816</t>
   </si>
   <si>
     <t>Enter Alternative Contact Perosn</t>
@@ -127,7 +127,7 @@
     <t>Scroll</t>
   </si>
   <si>
-    <t>Nationality*'</t>
+    <t>Scrollup</t>
   </si>
   <si>
     <t>Gender</t>
@@ -205,7 +205,7 @@
     <t>Camera</t>
   </si>
   <si>
-    <t>CHOOSE PAN</t>
+    <t>Continue</t>
   </si>
   <si>
     <t>Pan no</t>
@@ -232,10 +232,19 @@
     <t>className = android.widget.CheckBox</t>
   </si>
   <si>
-    <t>Continue</t>
-  </si>
-  <si>
     <t>xpath = //android.widget.Button[@content-desc="Continue"]</t>
+  </si>
+  <si>
+    <t>Verify Test</t>
+  </si>
+  <si>
+    <t>xpath =  //android.view.View[@content-desc="Verify Mobile Number"]</t>
+  </si>
+  <si>
+    <t>Verify</t>
+  </si>
+  <si>
+    <t>Verify Mobile Number</t>
   </si>
 </sst>
 </file>
@@ -243,10 +252,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -285,6 +294,50 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -293,18 +346,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -316,19 +378,26 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -341,67 +410,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -429,181 +438,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -652,16 +661,40 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -683,6 +716,17 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
@@ -691,51 +735,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -754,149 +763,149 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -938,7 +947,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
@@ -1263,10 +1272,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="6"/>
@@ -1274,7 +1283,7 @@
     <col min="1" max="1" width="14.4285714285714" customWidth="1"/>
     <col min="2" max="2" width="30.2857142857143" customWidth="1"/>
     <col min="3" max="3" width="33" customWidth="1"/>
-    <col min="4" max="4" width="70" style="1" customWidth="1"/>
+    <col min="4" max="4" width="74.7809523809524" style="1" customWidth="1"/>
     <col min="5" max="5" width="18.1428571428571" customWidth="1"/>
     <col min="6" max="6" width="65.5714285714286" customWidth="1"/>
     <col min="7" max="7" width="15.8571428571429" customWidth="1"/>
@@ -1502,10 +1511,10 @@
         <v>11</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" s="15" t="s">
         <v>37</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1702,7 +1711,7 @@
         <v>11</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>63</v>
@@ -1796,16 +1805,36 @@
         <v>7</v>
       </c>
       <c r="C26" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26" s="14" t="s">
         <v>72</v>
-      </c>
-      <c r="D26" s="14" t="s">
-        <v>73</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>10</v>
       </c>
       <c r="F26" s="8" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>